<commit_message>
changes in file a
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/NewStudents.xlsx
+++ b/src/test/resources/Excel/NewStudents.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>StudentName</t>
   </si>
@@ -306,6 +306,96 @@
   </si>
   <si>
     <t>AD5320</t>
+  </si>
+  <si>
+    <t>Kilback Satterfield</t>
+  </si>
+  <si>
+    <t>Adolfo</t>
+  </si>
+  <si>
+    <t>5860732332</t>
+  </si>
+  <si>
+    <t>5948266638</t>
+  </si>
+  <si>
+    <t>KilbackSatterfield@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9849</t>
+  </si>
+  <si>
+    <t>Waters Beer</t>
+  </si>
+  <si>
+    <t>Earline</t>
+  </si>
+  <si>
+    <t>3635531881</t>
+  </si>
+  <si>
+    <t>4454075079</t>
+  </si>
+  <si>
+    <t>WatersBeer@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD7047</t>
+  </si>
+  <si>
+    <t>Gottlieb Kessler</t>
+  </si>
+  <si>
+    <t>Maritza</t>
+  </si>
+  <si>
+    <t>3483563899</t>
+  </si>
+  <si>
+    <t>3156645634</t>
+  </si>
+  <si>
+    <t>GottliebKessler@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD8870</t>
+  </si>
+  <si>
+    <t>Lang Bernhard</t>
+  </si>
+  <si>
+    <t>Dale</t>
+  </si>
+  <si>
+    <t>7664871913</t>
+  </si>
+  <si>
+    <t>8189668962</t>
+  </si>
+  <si>
+    <t>LangBernhard@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3067</t>
+  </si>
+  <si>
+    <t>Schumm Heidenreich</t>
+  </si>
+  <si>
+    <t>Titus</t>
+  </si>
+  <si>
+    <t>8963008534</t>
+  </si>
+  <si>
+    <t>5046953430</t>
+  </si>
+  <si>
+    <t>SchummHeidenreich@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5644</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1555,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -1795,6 +1885,106 @@
         <v>92</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fixed flow of new student
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/NewStudents.xlsx
+++ b/src/test/resources/Excel/NewStudents.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
   <si>
     <t>StudentName</t>
   </si>
@@ -774,6 +774,348 @@
   </si>
   <si>
     <t>AD2316</t>
+  </si>
+  <si>
+    <t>Kessler Runte</t>
+  </si>
+  <si>
+    <t>Olin</t>
+  </si>
+  <si>
+    <t>6414338856</t>
+  </si>
+  <si>
+    <t>9393812098</t>
+  </si>
+  <si>
+    <t>KesslerRunte@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD2646</t>
+  </si>
+  <si>
+    <t>Howell Koelpin</t>
+  </si>
+  <si>
+    <t>Ed</t>
+  </si>
+  <si>
+    <t>9575201245</t>
+  </si>
+  <si>
+    <t>8706760528</t>
+  </si>
+  <si>
+    <t>HowellKoelpin@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9829</t>
+  </si>
+  <si>
+    <t>Hills Watsica</t>
+  </si>
+  <si>
+    <t>Rupert</t>
+  </si>
+  <si>
+    <t>6449026896</t>
+  </si>
+  <si>
+    <t>5378548338</t>
+  </si>
+  <si>
+    <t>HillsWatsica@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9378</t>
+  </si>
+  <si>
+    <t>Botsford Littel</t>
+  </si>
+  <si>
+    <t>Winford</t>
+  </si>
+  <si>
+    <t>8486967261</t>
+  </si>
+  <si>
+    <t>5503420437</t>
+  </si>
+  <si>
+    <t>BotsfordLittel@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD2180</t>
+  </si>
+  <si>
+    <t>Turcotte Kuhlman</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>8668617344</t>
+  </si>
+  <si>
+    <t>7609915767</t>
+  </si>
+  <si>
+    <t>TurcotteKuhlman@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9518</t>
+  </si>
+  <si>
+    <t>Altenwerth Sipes</t>
+  </si>
+  <si>
+    <t>Jeannine</t>
+  </si>
+  <si>
+    <t>9732936558</t>
+  </si>
+  <si>
+    <t>6084743216</t>
+  </si>
+  <si>
+    <t>AltenwerthSipes@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD1857</t>
+  </si>
+  <si>
+    <t>Nienow Green</t>
+  </si>
+  <si>
+    <t>Rodolfo</t>
+  </si>
+  <si>
+    <t>3194003211</t>
+  </si>
+  <si>
+    <t>3004825105</t>
+  </si>
+  <si>
+    <t>NienowGreen@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3722</t>
+  </si>
+  <si>
+    <t>Rolfson Wehner</t>
+  </si>
+  <si>
+    <t>Lyndon</t>
+  </si>
+  <si>
+    <t>5206075466</t>
+  </si>
+  <si>
+    <t>3670515960</t>
+  </si>
+  <si>
+    <t>RolfsonWehner@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3331</t>
+  </si>
+  <si>
+    <t>Wilkinson Koepp</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>5934780039</t>
+  </si>
+  <si>
+    <t>7728210581</t>
+  </si>
+  <si>
+    <t>WilkinsonKoepp@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9912</t>
+  </si>
+  <si>
+    <t>Cruickshank D'Amore</t>
+  </si>
+  <si>
+    <t>Delena</t>
+  </si>
+  <si>
+    <t>5212992532</t>
+  </si>
+  <si>
+    <t>6081417927</t>
+  </si>
+  <si>
+    <t>CruickshankD'Amore@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD6931</t>
+  </si>
+  <si>
+    <t>Rice Kub</t>
+  </si>
+  <si>
+    <t>Carli</t>
+  </si>
+  <si>
+    <t>5726536221</t>
+  </si>
+  <si>
+    <t>4596780178</t>
+  </si>
+  <si>
+    <t>RiceKub@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD8647</t>
+  </si>
+  <si>
+    <t>Nader Spencer</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>3453608322</t>
+  </si>
+  <si>
+    <t>5671299484</t>
+  </si>
+  <si>
+    <t>NaderSpencer@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD1108</t>
+  </si>
+  <si>
+    <t>Flatley McCullough</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>7340007559</t>
+  </si>
+  <si>
+    <t>4176087803</t>
+  </si>
+  <si>
+    <t>FlatleyMcCullough@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD6923</t>
+  </si>
+  <si>
+    <t>Renner Littel</t>
+  </si>
+  <si>
+    <t>Christinia</t>
+  </si>
+  <si>
+    <t>5697404055</t>
+  </si>
+  <si>
+    <t>3623957549</t>
+  </si>
+  <si>
+    <t>RennerLittel@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5805</t>
+  </si>
+  <si>
+    <t>Kerluke Tromp</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>3067104548</t>
+  </si>
+  <si>
+    <t>7530749469</t>
+  </si>
+  <si>
+    <t>KerlukeTromp@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD1604</t>
+  </si>
+  <si>
+    <t>Becker Rodriguez</t>
+  </si>
+  <si>
+    <t>Eloise</t>
+  </si>
+  <si>
+    <t>4374465510</t>
+  </si>
+  <si>
+    <t>3978001471</t>
+  </si>
+  <si>
+    <t>BeckerRodriguez@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD9714</t>
+  </si>
+  <si>
+    <t>Toy Dickens</t>
+  </si>
+  <si>
+    <t>Silas</t>
+  </si>
+  <si>
+    <t>4524178908</t>
+  </si>
+  <si>
+    <t>7130580017</t>
+  </si>
+  <si>
+    <t>ToyDickens@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3475</t>
+  </si>
+  <si>
+    <t>O'Conner Fisher</t>
+  </si>
+  <si>
+    <t>Dorie</t>
+  </si>
+  <si>
+    <t>5347643850</t>
+  </si>
+  <si>
+    <t>6211310336</t>
+  </si>
+  <si>
+    <t>O'ConnerFisher@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5529</t>
+  </si>
+  <si>
+    <t>Connelly Farrell</t>
+  </si>
+  <si>
+    <t>Theodore</t>
+  </si>
+  <si>
+    <t>3631752501</t>
+  </si>
+  <si>
+    <t>6181885702</t>
+  </si>
+  <si>
+    <t>ConnellyFarrell@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD1697</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +2275,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -2783,6 +3125,386 @@
         <v>248</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>251</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>265</v>
+      </c>
+      <c r="F47" t="s" s="0">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="F48" t="s" s="0">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>273</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>276</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>277</v>
+      </c>
+      <c r="F49" t="s" s="0">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>279</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>282</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="F50" t="s" s="0">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="F51" t="s" s="0">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="F52" t="s" s="0">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="F53" t="s" s="0">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="F54" t="s" s="0">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="F55" t="s" s="0">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="F56" t="s" s="0">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="F57" t="s" s="0">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="E58" t="s" s="0">
+        <v>331</v>
+      </c>
+      <c r="F58" t="s" s="0">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>333</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>336</v>
+      </c>
+      <c r="E59" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="F59" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>340</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="E60" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="F60" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>346</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="E61" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="F61" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>352</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>353</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>354</v>
+      </c>
+      <c r="E62" t="s" s="0">
+        <v>355</v>
+      </c>
+      <c r="F62" t="s" s="0">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>357</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>358</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>359</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>360</v>
+      </c>
+      <c r="E63" t="s" s="0">
+        <v>361</v>
+      </c>
+      <c r="F63" t="s" s="0">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fixed : Student flow completed
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/NewStudents.xlsx
+++ b/src/test/resources/Excel/NewStudents.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="404">
   <si>
     <t>StudentName</t>
   </si>
@@ -1116,6 +1116,129 @@
   </si>
   <si>
     <t>AD1697</t>
+  </si>
+  <si>
+    <t>Yost Gutkowski</t>
+  </si>
+  <si>
+    <t>Asa</t>
+  </si>
+  <si>
+    <t>7987444496</t>
+  </si>
+  <si>
+    <t>6941903893</t>
+  </si>
+  <si>
+    <t>YostGutkowski@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3196</t>
+  </si>
+  <si>
+    <t>Greenholt Friesen</t>
+  </si>
+  <si>
+    <t>6124914882</t>
+  </si>
+  <si>
+    <t>7206189218</t>
+  </si>
+  <si>
+    <t>GreenholtFriesen@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5395</t>
+  </si>
+  <si>
+    <t>Upton Runolfsdottir</t>
+  </si>
+  <si>
+    <t>Kati</t>
+  </si>
+  <si>
+    <t>7349724520</t>
+  </si>
+  <si>
+    <t>4985908368</t>
+  </si>
+  <si>
+    <t>UptonRunolfsdottir@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5222</t>
+  </si>
+  <si>
+    <t>Reynolds Carroll</t>
+  </si>
+  <si>
+    <t>Fleta</t>
+  </si>
+  <si>
+    <t>4802247669</t>
+  </si>
+  <si>
+    <t>9323330101</t>
+  </si>
+  <si>
+    <t>ReynoldsCarroll@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD1719</t>
+  </si>
+  <si>
+    <t>Rolfson Weber</t>
+  </si>
+  <si>
+    <t>Yen</t>
+  </si>
+  <si>
+    <t>4220748234</t>
+  </si>
+  <si>
+    <t>7478048067</t>
+  </si>
+  <si>
+    <t>RolfsonWeber@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD3024</t>
+  </si>
+  <si>
+    <t>Labadie Swift</t>
+  </si>
+  <si>
+    <t>Imogene</t>
+  </si>
+  <si>
+    <t>5966673372</t>
+  </si>
+  <si>
+    <t>5054900027</t>
+  </si>
+  <si>
+    <t>LabadieSwift@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD7495</t>
+  </si>
+  <si>
+    <t>Batz Abshire</t>
+  </si>
+  <si>
+    <t>Inge</t>
+  </si>
+  <si>
+    <t>5263937136</t>
+  </si>
+  <si>
+    <t>8007454009</t>
+  </si>
+  <si>
+    <t>BatzAbshire@yopmail.com</t>
+  </si>
+  <si>
+    <t>AD5866</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2398,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -3505,6 +3628,146 @@
         <v>362</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>366</v>
+      </c>
+      <c r="E64" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="F64" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>370</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="E65" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="F65" t="s" s="0">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>374</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>376</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="E66" t="s" s="0">
+        <v>378</v>
+      </c>
+      <c r="F66" t="s" s="0">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>380</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>382</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="E67" t="s" s="0">
+        <v>384</v>
+      </c>
+      <c r="F67" t="s" s="0">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>388</v>
+      </c>
+      <c r="D68" t="s" s="0">
+        <v>389</v>
+      </c>
+      <c r="E68" t="s" s="0">
+        <v>390</v>
+      </c>
+      <c r="F68" t="s" s="0">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>392</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>393</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>394</v>
+      </c>
+      <c r="D69" t="s" s="0">
+        <v>395</v>
+      </c>
+      <c r="E69" t="s" s="0">
+        <v>396</v>
+      </c>
+      <c r="F69" t="s" s="0">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>398</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>399</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>400</v>
+      </c>
+      <c r="D70" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="E70" t="s" s="0">
+        <v>402</v>
+      </c>
+      <c r="F70" t="s" s="0">
+        <v>403</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>